<commit_message>
Update Section Properties ITERATION007.xlsx
</commit_message>
<xml_diff>
--- a/src/Section Properties ITERATION007.xlsx
+++ b/src/Section Properties ITERATION007.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\y544q894\Documents\GitHub\structures-calc\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6331CA90-0FC3-442C-93CF-B4490C29F642}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B2535C-E576-4309-9180-997DC5DD7CCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -929,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AK25" sqref="AK25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AL16" sqref="AL16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3476,7 +3476,7 @@
         <v>1</v>
       </c>
       <c r="AL15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AO15" t="s">
         <v>62</v>

</xml_diff>